<commit_message>
Big changes. Bar plot w/ highlighting when mouseover brain; plots are centered; modified database and brain svg to have identical area names
</commit_message>
<xml_diff>
--- a/WM_StudyDatabase.xlsx
+++ b/WM_StudyDatabase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35940" yWindow="1060" windowWidth="32580" windowHeight="21120" tabRatio="500"/>
+    <workbookView xWindow="16580" yWindow="0" windowWidth="32580" windowHeight="21120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,12 +61,6 @@
     <t>8r</t>
   </si>
   <si>
-    <t>9/46d</t>
-  </si>
-  <si>
-    <t>9/46v</t>
-  </si>
-  <si>
     <t>Core</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>Perirhinal</t>
   </si>
   <si>
-    <t>S2</t>
-  </si>
-  <si>
     <t>STPc</t>
   </si>
   <si>
@@ -124,12 +115,6 @@
     <t>Temporal Pole</t>
   </si>
   <si>
-    <t>TEam a</t>
-  </si>
-  <si>
-    <t>TEam p</t>
-  </si>
-  <si>
     <t>TEad</t>
   </si>
   <si>
@@ -154,21 +139,12 @@
     <t>Superior Colliculus</t>
   </si>
   <si>
-    <t>Mediodorsal nucleus of thalamus</t>
-  </si>
-  <si>
-    <t>Ventral posterior lateral nucleus of thalamus</t>
-  </si>
-  <si>
     <t>Caudate nucleus</t>
   </si>
   <si>
     <t>Hippocampus</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t>Authors</t>
   </si>
   <si>
@@ -178,12 +154,6 @@
     <t>Journal</t>
   </si>
   <si>
-    <t>Positive Finding</t>
-  </si>
-  <si>
-    <t>Negative Finding</t>
-  </si>
-  <si>
     <t>2,3,4,5</t>
   </si>
   <si>
@@ -3878,6 +3848,36 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>TEa-ma</t>
+  </si>
+  <si>
+    <t>TEa-mp</t>
+  </si>
+  <si>
+    <t>negative_finding</t>
+  </si>
+  <si>
+    <t>positive_finding</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>VPL nucl. of thalamus</t>
+  </si>
+  <si>
+    <t>MD nucl. of thalamus</t>
+  </si>
+  <si>
+    <t>9-46d</t>
+  </si>
+  <si>
+    <t>9-46v</t>
   </si>
 </sst>
 </file>
@@ -3970,7 +3970,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4004,6 +4004,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -4360,8 +4363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4373,13 +4376,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>199</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>198</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4396,7 +4399,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" s="5">
         <v>6</v>
@@ -4407,7 +4410,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -4416,7 +4419,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C5" s="5">
         <v>6</v>
@@ -4427,7 +4430,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5">
         <v>6</v>
@@ -4439,7 +4442,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4447,7 +4450,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -4456,7 +4459,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -4465,7 +4468,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -4474,7 +4477,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -4486,7 +4489,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4495,7 +4498,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4503,7 +4506,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -4512,7 +4515,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -4521,7 +4524,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -4530,7 +4533,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -4548,7 +4551,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C19" s="5">
         <v>47</v>
@@ -4559,7 +4562,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -4568,7 +4571,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -4577,7 +4580,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -4586,7 +4589,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -4601,41 +4604,41 @@
     </row>
     <row r="25" spans="1:4" ht="60">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>202</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>203</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B27" s="5">
         <v>63</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B28" s="5">
         <v>67</v>
@@ -4644,25 +4647,25 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" s="5">
         <v>71</v>
@@ -4671,34 +4674,34 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B35" s="5">
         <v>65</v>
@@ -4707,16 +4710,16 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B37" s="5">
         <v>27</v>
@@ -4727,16 +4730,16 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B39" s="5">
         <v>84</v>
@@ -4745,16 +4748,16 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>194</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B41" s="5">
         <v>63</v>
@@ -4763,7 +4766,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B42" s="5">
         <v>63</v>
@@ -4772,7 +4775,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B43" s="5">
         <v>63</v>
@@ -4781,16 +4784,16 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B45" s="5">
         <v>84</v>
@@ -4800,29 +4803,29 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
-        <v>34</v>
+      <c r="A46" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
-        <v>35</v>
+      <c r="A47" s="12" t="s">
+        <v>196</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C48" s="5">
         <v>94</v>
@@ -4830,38 +4833,38 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B52" s="5">
         <v>99</v>
@@ -4870,18 +4873,18 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B54" s="5">
         <v>60</v>
@@ -4890,25 +4893,25 @@
     </row>
     <row r="55" spans="1:3" ht="30">
       <c r="A55" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="30">
       <c r="A56" s="1" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="B56" s="5">
         <v>108</v>
       </c>
       <c r="C56" s="5"/>
     </row>
-    <row r="57" spans="1:3" ht="45">
+    <row r="57" spans="1:3" ht="30">
       <c r="A57" s="1" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5">
@@ -4917,7 +4920,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B58" s="5">
         <v>110</v>
@@ -4926,10 +4929,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C59" s="5"/>
     </row>
@@ -4959,22 +4962,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30">
       <c r="A1" s="10" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4985,7 +4988,7 @@
         <v>2010</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4993,7 +4996,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5001,7 +5004,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5009,7 +5012,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5017,7 +5020,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5025,7 +5028,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5033,7 +5036,7 @@
         <v>7</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5041,7 +5044,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5049,7 +5052,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5057,7 +5060,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5065,7 +5068,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5073,7 +5076,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5081,7 +5084,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -5089,7 +5092,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -5097,7 +5100,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5105,7 +5108,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5113,7 +5116,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5121,7 +5124,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5129,7 +5132,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -5137,7 +5140,7 @@
         <v>20</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -5145,7 +5148,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -5153,7 +5156,7 @@
         <v>22</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -5161,7 +5164,7 @@
         <v>23</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -5169,7 +5172,7 @@
         <v>24</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5177,7 +5180,7 @@
         <v>25</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -5185,7 +5188,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5193,7 +5196,7 @@
         <v>27</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5201,7 +5204,7 @@
         <v>28</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5209,7 +5212,7 @@
         <v>29</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5217,7 +5220,7 @@
         <v>30</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5225,7 +5228,7 @@
         <v>31</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5233,7 +5236,7 @@
         <v>32</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5241,7 +5244,7 @@
         <v>33</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5249,7 +5252,7 @@
         <v>34</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5257,7 +5260,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5265,7 +5268,7 @@
         <v>36</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5273,7 +5276,7 @@
         <v>37</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5281,7 +5284,7 @@
         <v>38</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5289,7 +5292,7 @@
         <v>39</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -5297,7 +5300,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -5305,7 +5308,7 @@
         <v>41</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -5313,7 +5316,7 @@
         <v>42</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -5321,7 +5324,7 @@
         <v>43</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -5329,7 +5332,7 @@
         <v>44</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -5337,7 +5340,7 @@
         <v>45</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -5345,7 +5348,7 @@
         <v>46</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -5353,7 +5356,7 @@
         <v>47</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -5361,7 +5364,7 @@
         <v>48</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -5369,7 +5372,7 @@
         <v>49</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -5377,7 +5380,7 @@
         <v>50</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -5385,7 +5388,7 @@
         <v>51</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -5393,7 +5396,7 @@
         <v>52</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -5401,7 +5404,7 @@
         <v>53</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -5409,7 +5412,7 @@
         <v>54</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -5417,7 +5420,7 @@
         <v>55</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -5425,7 +5428,7 @@
         <v>56</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -5433,7 +5436,7 @@
         <v>57</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -5441,7 +5444,7 @@
         <v>58</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -5449,7 +5452,7 @@
         <v>59</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -5457,7 +5460,7 @@
         <v>60</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -5465,7 +5468,7 @@
         <v>61</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -5473,7 +5476,7 @@
         <v>62</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -5481,7 +5484,7 @@
         <v>63</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -5489,7 +5492,7 @@
         <v>64</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -5497,7 +5500,7 @@
         <v>65</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -5505,7 +5508,7 @@
         <v>66</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -5513,7 +5516,7 @@
         <v>67</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -5521,7 +5524,7 @@
         <v>68</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -5529,7 +5532,7 @@
         <v>69</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -5537,7 +5540,7 @@
         <v>70</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -5545,7 +5548,7 @@
         <v>71</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -5553,7 +5556,7 @@
         <v>72</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -5561,7 +5564,7 @@
         <v>73</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -5569,7 +5572,7 @@
         <v>74</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -5577,7 +5580,7 @@
         <v>75</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -5585,7 +5588,7 @@
         <v>76</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -5593,7 +5596,7 @@
         <v>77</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -5601,7 +5604,7 @@
         <v>78</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -5609,7 +5612,7 @@
         <v>79</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -5617,7 +5620,7 @@
         <v>80</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -5625,7 +5628,7 @@
         <v>81</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -5633,7 +5636,7 @@
         <v>82</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -5641,7 +5644,7 @@
         <v>83</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -5649,7 +5652,7 @@
         <v>84</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -5657,7 +5660,7 @@
         <v>85</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -5665,7 +5668,7 @@
         <v>86</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -5673,7 +5676,7 @@
         <v>87</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -5681,7 +5684,7 @@
         <v>88</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -5689,7 +5692,7 @@
         <v>89</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -5697,7 +5700,7 @@
         <v>90</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -5705,7 +5708,7 @@
         <v>91</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -5713,7 +5716,7 @@
         <v>92</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -5721,7 +5724,7 @@
         <v>93</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -5729,7 +5732,7 @@
         <v>94</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -5737,7 +5740,7 @@
         <v>95</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -5745,7 +5748,7 @@
         <v>96</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -5753,7 +5756,7 @@
         <v>97</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -5761,7 +5764,7 @@
         <v>98</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -5769,7 +5772,7 @@
         <v>99</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -5777,7 +5780,7 @@
         <v>100</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -5785,7 +5788,7 @@
         <v>101</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -5793,7 +5796,7 @@
         <v>102</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -5801,7 +5804,7 @@
         <v>103</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -5809,7 +5812,7 @@
         <v>104</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -5817,7 +5820,7 @@
         <v>105</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -5825,7 +5828,7 @@
         <v>106</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -5833,7 +5836,7 @@
         <v>107</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -5841,7 +5844,7 @@
         <v>108</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -5849,7 +5852,7 @@
         <v>109</v>
       </c>
       <c r="G110" s="9" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -5857,7 +5860,7 @@
         <v>110</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced spaces in area names with underscores, and fixed names displayed in plot
</commit_message>
<xml_diff>
--- a/WM_StudyDatabase.xlsx
+++ b/WM_StudyDatabase.xlsx
@@ -112,9 +112,6 @@
     <t>Subiculum</t>
   </si>
   <si>
-    <t>Temporal Pole</t>
-  </si>
-  <si>
     <t>TEad</t>
   </si>
   <si>
@@ -136,12 +133,6 @@
     <t>VIP</t>
   </si>
   <si>
-    <t>Superior Colliculus</t>
-  </si>
-  <si>
-    <t>Caudate nucleus</t>
-  </si>
-  <si>
     <t>Hippocampus</t>
   </si>
   <si>
@@ -3859,25 +3850,34 @@
     <t>TEa-mp</t>
   </si>
   <si>
-    <t>negative_finding</t>
-  </si>
-  <si>
-    <t>positive_finding</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
-    <t>VPL nucl. of thalamus</t>
-  </si>
-  <si>
-    <t>MD nucl. of thalamus</t>
-  </si>
-  <si>
     <t>9-46d</t>
   </si>
   <si>
     <t>9-46v</t>
+  </si>
+  <si>
+    <t>Temporal_Pole</t>
+  </si>
+  <si>
+    <t>Superior_Colliculus</t>
+  </si>
+  <si>
+    <t>MD_nucl_of_thalamus</t>
+  </si>
+  <si>
+    <t>VPL_nucl_of_thalamus</t>
+  </si>
+  <si>
+    <t>Caudate_nucleus</t>
+  </si>
+  <si>
+    <t>positive_findings</t>
+  </si>
+  <si>
+    <t>negative_findings</t>
   </si>
 </sst>
 </file>
@@ -4363,8 +4363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4376,13 +4376,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4399,7 +4399,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5">
         <v>6</v>
@@ -4410,7 +4410,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -4419,7 +4419,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" s="5">
         <v>6</v>
@@ -4430,7 +4430,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5">
         <v>6</v>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4450,7 +4450,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -4459,7 +4459,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -4468,7 +4468,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -4477,7 +4477,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -4489,7 +4489,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4498,7 +4498,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4506,7 +4506,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -4515,7 +4515,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -4524,7 +4524,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -4533,7 +4533,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -4551,7 +4551,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C19" s="5">
         <v>47</v>
@@ -4562,7 +4562,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -4571,7 +4571,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -4580,7 +4580,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -4589,7 +4589,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -4604,24 +4604,24 @@
     </row>
     <row r="25" spans="1:4" ht="60">
       <c r="A25" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60">
       <c r="A26" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D26" s="4"/>
     </row>
@@ -4633,7 +4633,7 @@
         <v>63</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4650,7 +4650,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C29" s="5"/>
     </row>
@@ -4659,7 +4659,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -4677,7 +4677,7 @@
         <v>18</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" s="5"/>
     </row>
@@ -4686,7 +4686,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C33" s="5"/>
     </row>
@@ -4695,7 +4695,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C34" s="5"/>
     </row>
@@ -4713,7 +4713,7 @@
         <v>22</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C36" s="5"/>
     </row>
@@ -4734,7 +4734,7 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -4748,10 +4748,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C40" s="5"/>
     </row>
@@ -4787,13 +4787,13 @@
         <v>29</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>30</v>
+        <v>197</v>
       </c>
       <c r="B45" s="5">
         <v>84</v>
@@ -4804,28 +4804,28 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C48" s="5">
         <v>94</v>
@@ -4833,38 +4833,38 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B52" s="5">
         <v>99</v>
@@ -4873,18 +4873,18 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="5">
         <v>60</v>
@@ -4893,16 +4893,16 @@
     </row>
     <row r="55" spans="1:3" ht="30">
       <c r="A55" s="4" t="s">
-        <v>38</v>
+        <v>198</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="30">
       <c r="A56" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B56" s="5">
         <v>108</v>
@@ -4920,7 +4920,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="B58" s="5">
         <v>110</v>
@@ -4929,10 +4929,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C59" s="5"/>
     </row>
@@ -4962,22 +4962,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="30">
       <c r="A1" s="10" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -4988,7 +4988,7 @@
         <v>2010</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4996,7 +4996,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5004,7 +5004,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5012,7 +5012,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5020,7 +5020,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5028,7 +5028,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5036,7 +5036,7 @@
         <v>7</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5044,7 +5044,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5052,7 +5052,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5060,7 +5060,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5068,7 +5068,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5076,7 +5076,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5084,7 +5084,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -5092,7 +5092,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -5100,7 +5100,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5108,7 +5108,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5116,7 +5116,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5124,7 +5124,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5132,7 +5132,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -5140,7 +5140,7 @@
         <v>20</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -5148,7 +5148,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -5156,7 +5156,7 @@
         <v>22</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -5164,7 +5164,7 @@
         <v>23</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -5172,7 +5172,7 @@
         <v>24</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5180,7 +5180,7 @@
         <v>25</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -5188,7 +5188,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5196,7 +5196,7 @@
         <v>27</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5204,7 +5204,7 @@
         <v>28</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5212,7 +5212,7 @@
         <v>29</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5220,7 +5220,7 @@
         <v>30</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5228,7 +5228,7 @@
         <v>31</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5236,7 +5236,7 @@
         <v>32</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5244,7 +5244,7 @@
         <v>33</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5252,7 +5252,7 @@
         <v>34</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5260,7 +5260,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5268,7 +5268,7 @@
         <v>36</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5276,7 +5276,7 @@
         <v>37</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5284,7 +5284,7 @@
         <v>38</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5292,7 +5292,7 @@
         <v>39</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -5300,7 +5300,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -5308,7 +5308,7 @@
         <v>41</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -5316,7 +5316,7 @@
         <v>42</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -5324,7 +5324,7 @@
         <v>43</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -5332,7 +5332,7 @@
         <v>44</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -5340,7 +5340,7 @@
         <v>45</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -5348,7 +5348,7 @@
         <v>46</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -5356,7 +5356,7 @@
         <v>47</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -5364,7 +5364,7 @@
         <v>48</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -5372,7 +5372,7 @@
         <v>49</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -5380,7 +5380,7 @@
         <v>50</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -5388,7 +5388,7 @@
         <v>51</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -5396,7 +5396,7 @@
         <v>52</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -5404,7 +5404,7 @@
         <v>53</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -5412,7 +5412,7 @@
         <v>54</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -5420,7 +5420,7 @@
         <v>55</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -5428,7 +5428,7 @@
         <v>56</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -5436,7 +5436,7 @@
         <v>57</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -5444,7 +5444,7 @@
         <v>58</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -5452,7 +5452,7 @@
         <v>59</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -5460,7 +5460,7 @@
         <v>60</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -5468,7 +5468,7 @@
         <v>61</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -5476,7 +5476,7 @@
         <v>62</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -5484,7 +5484,7 @@
         <v>63</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -5492,7 +5492,7 @@
         <v>64</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -5500,7 +5500,7 @@
         <v>65</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -5508,7 +5508,7 @@
         <v>66</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -5516,7 +5516,7 @@
         <v>67</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -5524,7 +5524,7 @@
         <v>68</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -5532,7 +5532,7 @@
         <v>69</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -5540,7 +5540,7 @@
         <v>70</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -5548,7 +5548,7 @@
         <v>71</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -5556,7 +5556,7 @@
         <v>72</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -5564,7 +5564,7 @@
         <v>73</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -5572,7 +5572,7 @@
         <v>74</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -5580,7 +5580,7 @@
         <v>75</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -5588,7 +5588,7 @@
         <v>76</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -5596,7 +5596,7 @@
         <v>77</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -5604,7 +5604,7 @@
         <v>78</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -5612,7 +5612,7 @@
         <v>79</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -5620,7 +5620,7 @@
         <v>80</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -5628,7 +5628,7 @@
         <v>81</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -5636,7 +5636,7 @@
         <v>82</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -5644,7 +5644,7 @@
         <v>83</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -5652,7 +5652,7 @@
         <v>84</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -5660,7 +5660,7 @@
         <v>85</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -5668,7 +5668,7 @@
         <v>86</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -5676,7 +5676,7 @@
         <v>87</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -5684,7 +5684,7 @@
         <v>88</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -5692,7 +5692,7 @@
         <v>89</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -5700,7 +5700,7 @@
         <v>90</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -5708,7 +5708,7 @@
         <v>91</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -5716,7 +5716,7 @@
         <v>92</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -5724,7 +5724,7 @@
         <v>93</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -5732,7 +5732,7 @@
         <v>94</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -5740,7 +5740,7 @@
         <v>95</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -5748,7 +5748,7 @@
         <v>96</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -5756,7 +5756,7 @@
         <v>97</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -5764,7 +5764,7 @@
         <v>98</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -5772,7 +5772,7 @@
         <v>99</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -5780,7 +5780,7 @@
         <v>100</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -5788,7 +5788,7 @@
         <v>101</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -5796,7 +5796,7 @@
         <v>102</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -5804,7 +5804,7 @@
         <v>103</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -5812,7 +5812,7 @@
         <v>104</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -5820,7 +5820,7 @@
         <v>105</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -5828,7 +5828,7 @@
         <v>106</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -5836,7 +5836,7 @@
         <v>107</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -5844,7 +5844,7 @@
         <v>108</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -5852,7 +5852,7 @@
         <v>109</v>
       </c>
       <c r="G110" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -5860,7 +5860,7 @@
         <v>110</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added references, bar plot links to references on click
</commit_message>
<xml_diff>
--- a/WM_StudyDatabase.xlsx
+++ b/WM_StudyDatabase.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16580" yWindow="0" windowWidth="32580" windowHeight="21120" tabRatio="500"/>
+    <workbookView xWindow="16580" yWindow="0" windowWidth="32580" windowHeight="21120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="206">
   <si>
     <t>24a</t>
   </si>
@@ -103,9 +104,6 @@
     <t>STPc</t>
   </si>
   <si>
-    <t>STPl</t>
-  </si>
-  <si>
     <t>STPr</t>
   </si>
   <si>
@@ -3878,6 +3876,15 @@
   </si>
   <si>
     <t>negative_findings</t>
+  </si>
+  <si>
+    <t>STPi</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>reference_number</t>
   </si>
 </sst>
 </file>
@@ -3945,8 +3952,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4009,7 +4018,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4021,6 +4030,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4032,6 +4042,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4363,8 +4374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4376,13 +4387,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4399,7 +4410,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="5">
         <v>6</v>
@@ -4410,7 +4421,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -4419,7 +4430,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5">
         <v>6</v>
@@ -4430,7 +4441,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5">
         <v>6</v>
@@ -4442,7 +4453,7 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4450,7 +4461,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -4459,7 +4470,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -4468,7 +4479,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -4477,7 +4488,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -4489,7 +4500,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -4498,7 +4509,7 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -4506,7 +4517,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="5"/>
     </row>
@@ -4515,7 +4526,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -4524,7 +4535,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="5"/>
     </row>
@@ -4533,7 +4544,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -4551,7 +4562,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5">
         <v>47</v>
@@ -4562,7 +4573,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -4571,7 +4582,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -4580,7 +4591,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -4589,7 +4600,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -4604,24 +4615,24 @@
     </row>
     <row r="25" spans="1:4" ht="60">
       <c r="A25" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="60">
       <c r="A26" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="D26" s="4"/>
     </row>
@@ -4633,7 +4644,7 @@
         <v>63</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -4650,7 +4661,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="5"/>
     </row>
@@ -4659,7 +4670,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -4677,7 +4688,7 @@
         <v>18</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="5"/>
     </row>
@@ -4686,7 +4697,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="5"/>
     </row>
@@ -4695,7 +4706,7 @@
         <v>20</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="5"/>
     </row>
@@ -4713,7 +4724,7 @@
         <v>22</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" s="5"/>
     </row>
@@ -4734,7 +4745,7 @@
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -4748,10 +4759,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" s="5"/>
     </row>
@@ -4766,7 +4777,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
       <c r="B42" s="5">
         <v>63</v>
@@ -4775,7 +4786,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B43" s="5">
         <v>63</v>
@@ -4784,16 +4795,16 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B45" s="5">
         <v>84</v>
@@ -4804,28 +4815,28 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="5">
         <v>94</v>
@@ -4833,38 +4844,38 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B52" s="5">
         <v>99</v>
@@ -4873,18 +4884,18 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B54" s="5">
         <v>60</v>
@@ -4893,16 +4904,16 @@
     </row>
     <row r="55" spans="1:3" ht="30">
       <c r="A55" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="30">
       <c r="A56" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B56" s="5">
         <v>108</v>
@@ -4911,7 +4922,7 @@
     </row>
     <row r="57" spans="1:3" ht="30">
       <c r="A57" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5">
@@ -4920,7 +4931,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B58" s="5">
         <v>110</v>
@@ -4929,10 +4940,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="5"/>
     </row>
@@ -4955,40 +4966,37 @@
   <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7" ht="30">
       <c r="A1" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2010</v>
-      </c>
       <c r="G2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4996,7 +5004,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5004,7 +5012,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5012,7 +5020,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -5020,7 +5028,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -5028,7 +5036,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5036,7 +5044,7 @@
         <v>7</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -5044,7 +5052,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5052,7 +5060,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -5060,7 +5068,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5068,7 +5076,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5076,7 +5084,7 @@
         <v>12</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5084,7 +5092,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -5092,7 +5100,7 @@
         <v>14</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -5100,7 +5108,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -5108,7 +5116,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -5116,7 +5124,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -5124,7 +5132,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -5132,7 +5140,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -5140,7 +5148,7 @@
         <v>20</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -5148,7 +5156,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -5156,7 +5164,7 @@
         <v>22</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -5164,7 +5172,7 @@
         <v>23</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -5172,7 +5180,7 @@
         <v>24</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5180,7 +5188,7 @@
         <v>25</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -5188,7 +5196,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5196,7 +5204,7 @@
         <v>27</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5204,7 +5212,7 @@
         <v>28</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5212,7 +5220,7 @@
         <v>29</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5220,7 +5228,7 @@
         <v>30</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5228,7 +5236,7 @@
         <v>31</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5236,7 +5244,7 @@
         <v>32</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5244,7 +5252,7 @@
         <v>33</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5252,7 +5260,7 @@
         <v>34</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5260,7 +5268,7 @@
         <v>35</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5268,7 +5276,7 @@
         <v>36</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5276,7 +5284,7 @@
         <v>37</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5284,7 +5292,7 @@
         <v>38</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5292,7 +5300,7 @@
         <v>39</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -5300,7 +5308,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -5308,7 +5316,7 @@
         <v>41</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -5316,7 +5324,7 @@
         <v>42</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -5324,7 +5332,7 @@
         <v>43</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -5332,7 +5340,7 @@
         <v>44</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -5340,7 +5348,7 @@
         <v>45</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -5348,7 +5356,7 @@
         <v>46</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -5356,7 +5364,7 @@
         <v>47</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -5364,7 +5372,7 @@
         <v>48</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -5372,7 +5380,7 @@
         <v>49</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -5380,7 +5388,7 @@
         <v>50</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -5388,7 +5396,7 @@
         <v>51</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -5396,7 +5404,7 @@
         <v>52</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -5404,7 +5412,7 @@
         <v>53</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -5412,7 +5420,7 @@
         <v>54</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -5420,7 +5428,7 @@
         <v>55</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -5428,7 +5436,7 @@
         <v>56</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -5436,7 +5444,7 @@
         <v>57</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -5444,7 +5452,7 @@
         <v>58</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -5452,7 +5460,7 @@
         <v>59</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -5460,7 +5468,7 @@
         <v>60</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -5468,7 +5476,7 @@
         <v>61</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -5476,7 +5484,7 @@
         <v>62</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -5484,7 +5492,7 @@
         <v>63</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -5492,7 +5500,7 @@
         <v>64</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -5500,7 +5508,7 @@
         <v>65</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -5508,7 +5516,7 @@
         <v>66</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -5516,7 +5524,7 @@
         <v>67</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -5524,7 +5532,7 @@
         <v>68</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -5532,7 +5540,7 @@
         <v>69</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -5540,7 +5548,7 @@
         <v>70</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -5548,7 +5556,7 @@
         <v>71</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -5556,7 +5564,7 @@
         <v>72</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -5564,7 +5572,7 @@
         <v>73</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -5572,7 +5580,7 @@
         <v>74</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -5580,7 +5588,7 @@
         <v>75</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -5588,7 +5596,7 @@
         <v>76</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -5596,7 +5604,7 @@
         <v>77</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -5604,7 +5612,7 @@
         <v>78</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -5612,7 +5620,7 @@
         <v>79</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -5620,7 +5628,7 @@
         <v>80</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -5628,7 +5636,7 @@
         <v>81</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -5636,7 +5644,7 @@
         <v>82</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -5644,7 +5652,7 @@
         <v>83</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -5652,7 +5660,7 @@
         <v>84</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -5660,7 +5668,7 @@
         <v>85</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -5668,7 +5676,7 @@
         <v>86</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -5676,7 +5684,7 @@
         <v>87</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -5684,7 +5692,7 @@
         <v>88</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -5692,7 +5700,7 @@
         <v>89</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -5700,7 +5708,7 @@
         <v>90</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -5708,7 +5716,7 @@
         <v>91</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -5716,7 +5724,7 @@
         <v>92</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -5724,7 +5732,7 @@
         <v>93</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -5732,7 +5740,7 @@
         <v>94</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -5740,7 +5748,7 @@
         <v>95</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -5748,7 +5756,7 @@
         <v>96</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -5756,7 +5764,7 @@
         <v>97</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -5764,7 +5772,7 @@
         <v>98</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -5772,7 +5780,7 @@
         <v>99</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -5780,7 +5788,7 @@
         <v>100</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -5788,7 +5796,7 @@
         <v>101</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -5796,7 +5804,7 @@
         <v>102</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -5804,7 +5812,7 @@
         <v>103</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -5812,7 +5820,7 @@
         <v>104</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -5820,7 +5828,7 @@
         <v>105</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -5828,7 +5836,7 @@
         <v>106</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -5836,7 +5844,7 @@
         <v>107</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -5844,7 +5852,7 @@
         <v>108</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -5852,7 +5860,7 @@
         <v>109</v>
       </c>
       <c r="G110" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -5860,7 +5868,920 @@
         <v>110</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30">
+      <c r="A1" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="9">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="9">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="9">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="9">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="9">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="9">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="9">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="9">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="9">
+        <v>37</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="9">
+        <v>38</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="9">
+        <v>39</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="9">
+        <v>40</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="9">
+        <v>41</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="9">
+        <v>42</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="9">
+        <v>43</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="9">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="9">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="9">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="9">
+        <v>47</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="9">
+        <v>48</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="9">
+        <v>49</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="9">
+        <v>50</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="9">
+        <v>51</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="9">
+        <v>52</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="9">
+        <v>53</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="9">
+        <v>54</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="9">
+        <v>55</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="9">
+        <v>56</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="9">
+        <v>57</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="9">
+        <v>58</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="9">
+        <v>59</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="9">
+        <v>60</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="9">
+        <v>61</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="9">
+        <v>62</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="9">
+        <v>63</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="9">
+        <v>64</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="9">
+        <v>65</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="9">
+        <v>66</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="9">
+        <v>67</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="9">
+        <v>68</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="9">
+        <v>69</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="9">
+        <v>70</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="9">
+        <v>71</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="9">
+        <v>72</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="9">
+        <v>73</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="9">
+        <v>74</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="9">
+        <v>75</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="9">
+        <v>76</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="9">
+        <v>77</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="9">
+        <v>78</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="9">
+        <v>79</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="9">
+        <v>80</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="9">
+        <v>81</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="9">
+        <v>82</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="9">
+        <v>83</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="9">
+        <v>84</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="9">
+        <v>85</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="9">
+        <v>86</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="9">
+        <v>87</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="9">
+        <v>88</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="9">
+        <v>89</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="9">
+        <v>90</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="9">
+        <v>91</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="9">
+        <v>92</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="9">
+        <v>93</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="9">
+        <v>94</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="9">
+        <v>95</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="9">
+        <v>96</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="9">
+        <v>97</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="9">
+        <v>98</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="9">
+        <v>99</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="9">
+        <v>100</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="9">
+        <v>101</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="9">
+        <v>102</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="9">
+        <v>103</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="9">
+        <v>104</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="9">
+        <v>105</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="9">
+        <v>106</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="9">
+        <v>107</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="9">
+        <v>108</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="9">
+        <v>109</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="9">
+        <v>110</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>